<commit_message>
Adaptacion a plataforma de gestion de dispositivos
Cambios:
-Elimina la necesidad d eacceder por HTTP a los dispositivos
-Buzon de peticiones MQTT
-Mucho mas.....
</commit_message>
<xml_diff>
--- a/src/Configuraciones/Riego/Secuenciador.xlsx
+++ b/src/Configuraciones/Riego/Secuenciador.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arduino\desarrollos\Sketchs\Riego\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlopezt\Documents\PlatformIO\Projects\Actuador-ESP32\src\Configuraciones\Riego\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF4304-00C2-47E7-BF58-A9B5A83F2DA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA33FD23-0F22-4D70-9D84-B15D98E7327E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E272C0E1-DFCC-4036-ADAB-96F87FDBC628}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E272C0E1-DFCC-4036-ADAB-96F87FDBC628}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Riego" sheetId="2" r:id="rId2"/>
+    <sheet name="Navidad" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +25,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="54">
   <si>
     <t>Intervalo</t>
   </si>
@@ -547,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5727D02F-810E-4AAF-AB01-9DED2FEDECD7}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
@@ -1817,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A576E3-0A24-417E-9C6A-D14CDB463C68}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20:D43"/>
     </sheetView>
   </sheetViews>
@@ -3466,4 +3472,1659 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E071485-F62F-4C4B-B8DC-1336AED995C7}">
+  <dimension ref="A1:AB43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:AB13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>+A2*5</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>+B2+4</f>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D13" si="0">+POWER(2,A2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B13" si="1">+A3*5</f>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="2">+B3+4</f>
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>+SUMPRODUCT($D$2:$D$13,E2:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:N14" si="3">+SUMPRODUCT($D$2:$D$13,F2:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>+SUMPRODUCT($D$2:$D$13,O2:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:X14" si="4">+SUMPRODUCT($D$2:$D$13,P2:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="4"/>
+        <v>4095</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="4"/>
+        <v>4095</v>
+      </c>
+      <c r="Y14">
+        <f>+SUMPRODUCT($D$2:$D$13,Y2:Y13)</f>
+        <v>4095</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" ref="Z14:AB14" si="5">+SUMPRODUCT($D$2:$D$13,Z2:Z13)</f>
+        <v>4095</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="5"/>
+        <v>4095</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="5"/>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <f>+E14</f>
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="str">
+        <f>+CONCATENATE(A20,B20,C20)</f>
+        <v>{"id":  0, "valor":0},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <f>+F14</f>
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" ref="D21:D43" si="6">+CONCATENATE(A21,B21,C21)</f>
+        <v>{"id":  1, "valor":0},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <f>+G14</f>
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  2, "valor":0},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <f>+H14</f>
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  3, "valor":0},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <f>+I14</f>
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  4, "valor":0},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <f>+J14</f>
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  5, "valor":0},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <f>+K14</f>
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  6, "valor":0},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <f>+L14</f>
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  7, "valor":0},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <f>+M14</f>
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  8, "valor":0},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <f>+N14</f>
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id":  9, "valor":0},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <f>+O14</f>
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 10, "valor":0},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <f>+P14</f>
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 11, "valor":0},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <f>+Q14</f>
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 12, "valor":0},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <f>+R14</f>
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 13, "valor":0},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <f>+S14</f>
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 14, "valor":0},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <f>+T14</f>
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 15, "valor":0},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <f>+U14</f>
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 16, "valor":0},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <f>+V14</f>
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 17, "valor":0},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <f>+W14</f>
+        <v>4095</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 18, "valor":4095},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <f>+X14</f>
+        <v>4095</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 19, "valor":4095},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <f>+Y14</f>
+        <v>4095</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 20, "valor":4095},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <f>+Z14</f>
+        <v>4095</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 21, "valor":4095},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <f>+AA14</f>
+        <v>4095</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 22, "valor":4095},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <f>+AB14</f>
+        <v>4095</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="6"/>
+        <v>{"id": 23, "valor":4095}</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>